<commit_message>
added a file and modified a file in the working directory
</commit_message>
<xml_diff>
--- a/Data Analysis/Excel/original-file.xlsx
+++ b/Data Analysis/Excel/original-file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HomePC\Desktop\Learning-Journey\Data Analysis\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74E89DB2-70C1-4709-B5BB-45F59FE714B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE86F90-093D-46E4-9E52-3817BF0324FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F511897E-5371-413D-A864-A392B88F2268}"/>
   </bookViews>
@@ -33,8 +33,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>EmployeeID</t>
   </si>
@@ -139,6 +161,9 @@
   </si>
   <si>
     <t>EndDate</t>
+  </si>
+  <si>
+    <t>LEN_LastName</t>
   </si>
 </sst>
 </file>
@@ -491,7 +516,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6379A4E6-10C7-4830-9E14-25F9B1DE3104}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
@@ -503,7 +528,7 @@
     <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -531,8 +556,11 @@
       <c r="I1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -560,8 +588,12 @@
       <c r="I2" s="1">
         <v>42253</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2" cm="1">
+        <f t="array" ref="J2:J10">LEN(C2:C10)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -589,8 +621,11 @@
       <c r="I3" s="1">
         <v>42287</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -618,8 +653,11 @@
       <c r="I4" s="1">
         <v>42986</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -647,8 +685,11 @@
       <c r="I5" s="1">
         <v>42341</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -676,8 +717,11 @@
       <c r="I6" s="1">
         <v>42977</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -705,8 +749,11 @@
       <c r="I7" s="1">
         <v>41528</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -734,8 +781,11 @@
       <c r="I8" s="1">
         <v>41551</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -763,8 +813,11 @@
       <c r="I9" s="1">
         <v>42116</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -791,6 +844,9 @@
       </c>
       <c r="I10" s="1">
         <v>40800</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>